<commit_message>
add README.md. Fix typos in DatabaseNormalization.xlsx
</commit_message>
<xml_diff>
--- a/DatabaseNormalization.xlsx
+++ b/DatabaseNormalization.xlsx
@@ -126,7 +126,7 @@
 - name2
 - phone
 - email
-It presumes these fields have implicit transitive dependencies, such that an update to a single field may require updates to fields for multiple stores in order to maintain consistency.
+It presumes these fields have implicit transitive dependencies, such that an update to a single field may require updates to fields for multiple stores in order to maintain consistency:
 - facebookUrl
 - mainImageUrl
 It presumes that `alternateImageUrl2` is a fallback URL for all stores that will be maintained in the constants table.</t>
@@ -170,7 +170,7 @@
     <t xml:space="preserve">This option corresponds to the following fields being dependent only on the store, despite some duplicate values among these fields: 
 - name
 - name2
-It presumes these fields have implicit transitive dependencies, such that an update to a single field may require updates to fields for multiple stores in order to maintain consistency.
+It presumes these fields have implicit transitive dependencies, such that an update to a single field may require updates to fields for multiple stores in order to maintain consistency:
 - phone
 - email
 - facebookUrl
@@ -207,7 +207,7 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">This option corresponds to the following fields having implicit transitive dependencies, such that an update to a single field may require updates to fields for multiple stores in order to maintain consistency.
+    <t xml:space="preserve">This option corresponds to the following fields having implicit transitive dependencies, such that an update to a single field may require updates to fields for multiple stores in order to maintain consistency:
 - name
 - name2
 - phone
@@ -246,7 +246,7 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">This option corresponds to the following fields having implicit transitive dependencies, such that an update to a single field may require updates to fields for multiple stores in order to maintain consistency.
+    <t xml:space="preserve">This option corresponds to the following fields having implicit transitive dependencies, such that an update to a single field may require updates to fields for multiple stores in order to maintain consistency:
 - name
 - facebookUrl
 - mainImageUrl
@@ -442,8 +442,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>322560</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1969560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -606,7 +606,7 @@
   <dimension ref="A2:A13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -690,7 +690,7 @@
   <dimension ref="A2:A17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -703,7 +703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="182.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="205.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -791,7 +791,7 @@
   <dimension ref="A2:A18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -902,7 +902,7 @@
   <dimension ref="A2:A20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1020,7 +1020,7 @@
   <dimension ref="A2:A20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>